<commit_message>
add VS CS  kind of characteristic
ajout CS VS et binding pour group.charasteristic.code 87d1dc9b3d813bd59d598d48747d22d4932dad66
</commit_message>
<xml_diff>
--- a/ig/sd-group-characteristic-alignement-vs/StructureDefinition-eclaire-group.xlsx
+++ b/ig/sd-group-characteristic-alignement-vs/StructureDefinition-eclaire-group.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="281">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-11T15:49:53+00:00</t>
+    <t>2024-01-10T17:41:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -736,7 +736,10 @@
     <t>Need a formal way of identifying the characteristic being described.</t>
   </si>
   <si>
-    <t>List of characteristics used to describe group members; e.g. gender, age, owner, location, etc.</t>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-group-characteristic-kind-vs</t>
   </si>
   <si>
     <t>Group.characteristic.value[x]</t>
@@ -772,9 +775,6 @@
   </si>
   <si>
     <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>extensible</t>
   </si>
   <si>
     <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-study-population-vs</t>
@@ -1225,8 +1225,8 @@
     <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="87.84765625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="75.2734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="81.36328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="82.8359375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -3699,13 +3699,11 @@
         <v>74</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="Y23" t="s" s="2">
         <v>231</v>
       </c>
+      <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>74</v>
@@ -3746,10 +3744,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3772,19 +3770,19 @@
         <v>74</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>74</v>
@@ -3812,7 +3810,7 @@
         <v>182</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>74</v>
@@ -3821,7 +3819,7 @@
         <v>74</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" t="s" s="2">
@@ -3831,7 +3829,7 @@
         <v>138</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>84</v>
@@ -3846,7 +3844,7 @@
         <v>97</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>74</v>
@@ -3854,13 +3852,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D25" t="s" s="2">
         <v>74</v>
@@ -3885,16 +3883,16 @@
         <v>178</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>74</v>
@@ -3919,7 +3917,7 @@
         <v>74</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="Y25" s="2"/>
       <c r="Z25" t="s" s="2">
@@ -3941,7 +3939,7 @@
         <v>74</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>84</v>
@@ -3956,7 +3954,7 @@
         <v>97</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>74</v>

</xml_diff>